<commit_message>
happy flow without pictures and opening hours
</commit_message>
<xml_diff>
--- a/RPA_Project_Googplace/Data/DataGoogleForms.xlsx
+++ b/RPA_Project_Googplace/Data/DataGoogleForms.xlsx
@@ -1,97 +1,116 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikim\Documents\GitHub\rpa_experiment\RPA_Project_Googplace\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57A28E2-861B-4898-9E6B-6829F7369631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FFAD7C-4C84-4F1B-8976-08D0F83EB42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{417F3AF6-5728-476F-A49D-DBD930158F9F}"/>
+    <workbookView xWindow="-28920" yWindow="-4695" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="DataGoogleForms" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+  <si>
+    <t>Timestamp</t>
+  </si>
   <si>
     <t>Firmenname</t>
   </si>
   <si>
+    <t>Kategorie</t>
+  </si>
+  <si>
+    <t>Standort</t>
+  </si>
+  <si>
+    <t>Adresse</t>
+  </si>
+  <si>
+    <t>PLZ</t>
+  </si>
+  <si>
+    <t>Stadt</t>
+  </si>
+  <si>
+    <t>Lieferdienst</t>
+  </si>
+  <si>
+    <t>Einzugsgebiete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falls Ihre Kunden Ihre Kontakttelefonnummer sehen sollen. </t>
+  </si>
+  <si>
+    <t>Vor- und Nachname</t>
+  </si>
+  <si>
     <t>Mailadresse</t>
   </si>
   <si>
     <t>Telefonnummer</t>
   </si>
   <si>
+    <t>2021/10/26 5:18:40 PM GMT+2</t>
+  </si>
+  <si>
+    <t>Mike's Test Daten</t>
+  </si>
+  <si>
+    <t>Anwalt</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Hauptstrasse 1</t>
+  </si>
+  <si>
+    <t>DÃ¼dingen</t>
+  </si>
+  <si>
+    <t>Gebiet 1</t>
+  </si>
+  <si>
+    <t>https://autonomous-stories.ch</t>
+  </si>
+  <si>
+    <t>Mike MÃ¼ller</t>
+  </si>
+  <si>
     <t>v1@test.ch</t>
   </si>
   <si>
-    <t>Virtuell2</t>
-  </si>
-  <si>
-    <t>v2@tech.ch</t>
-  </si>
-  <si>
-    <t>Virtuell1</t>
-  </si>
-  <si>
-    <t>Passwort</t>
-  </si>
-  <si>
-    <t>Rpa_1234</t>
-  </si>
-  <si>
-    <t>Vorname</t>
-  </si>
-  <si>
-    <t>Nachname</t>
-  </si>
-  <si>
-    <t>V1</t>
-  </si>
-  <si>
-    <t>RPA</t>
-  </si>
-  <si>
-    <t>V2</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>719711111</t>
-  </si>
-  <si>
-    <t>819712222</t>
+    <t>3186</t>
+  </si>
+  <si>
+    <t>765793701</t>
+  </si>
+  <si>
+    <t>Webseite</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>Das ist das tollste Unternehmen der Welt!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,23 +119,315 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -124,19 +435,205 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+  <cellStyles count="42">
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -447,85 +944,110 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{508554E8-C8A3-4096-B762-549CF05D61FD}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{597CB863-DAB4-4D74-8E37-06A95CC92ED1}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{53A65D77-BCAA-4CFE-AB39-924F264FB6CB}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>